<commit_message>
Implement limited unit check, exception clause, and reconfigure hourly check
</commit_message>
<xml_diff>
--- a/Continuous Execution/vft_config.xlsx
+++ b/Continuous Execution/vft_config.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SorinoSK\School\Internship\Work\IoT\automated_units_status\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[01] Laptop Files\[01] School Files\Internship\[01] Work\[01] IoT\[01] IoT Devices\[04] Intern-IoT-Automated-Daily-Status (Github)\Continuous Execution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665785E3-FFE9-4A78-9D8B-FDDF17024E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620393FE-2DFF-45A1-B4DA-227CB5C0EB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="6105" yWindow="1110" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
-    <sheet name="units_sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="account_sheet" sheetId="3" r:id="rId2"/>
-    <sheet name="data_sheet" sheetId="2" r:id="rId3"/>
-    <sheet name="email_sheet" sheetId="4" r:id="rId4"/>
+    <sheet name="closely_monitor_units_sheet" sheetId="5" r:id="rId1"/>
+    <sheet name="daily_report_units_sheet" sheetId="1" r:id="rId2"/>
+    <sheet name="account_sheet" sheetId="3" r:id="rId3"/>
+    <sheet name="data_sheet" sheetId="2" r:id="rId4"/>
+    <sheet name="email_sheet" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>5kW - Unit 1 Backup 2</t>
   </si>
@@ -642,13 +643,13 @@
     <t>RECIPIENTS_DAILY</t>
   </si>
   <si>
-    <t>vft.iot.test@gmail.com,
-sinkiat.seow@vflowtech.com, john.jacob@vflowtech.com,
-anhtrung.ta@vflowtech.com</t>
-  </si>
-  <si>
-    <t>vft.iot.test@gmail.com,
-sinkiat.seow@vflowtech.com, john.jacob@vflowtech.com, saravanan.sampath@vflowtech.com, hardik.kansara@vflowtech.com, sanjana.ramesh@vflowtech.com,
+    <t>sinkiat.seow@vflowtech.com</t>
+  </si>
+  <si>
+    <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com, saravanan.sampath@vflowtech.com, hardik.kansara@vflowtech.com, sanjana.ramesh@vflowtech.com, anhtrung.ta@vflowtech.com</t>
+  </si>
+  <si>
+    <t>vft.iot.test@gmail.com, john.jacob@vflowtech.com,
 anhtrung.ta@vflowtech.com</t>
   </si>
 </sst>
@@ -656,7 +657,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -710,6 +711,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -728,10 +737,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -760,8 +770,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1073,11 +1090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2916DAA6-D9E6-4FF8-8C3E-F0600BF95911}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1109,152 +1126,66 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3">
-        <v>28</v>
+        <v>363</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3">
-        <v>71</v>
+        <v>390</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3">
-        <v>331</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3">
-        <v>332</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3">
-        <v>363</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3">
-        <v>390</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3">
-        <v>439</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3">
-        <v>412</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3">
-        <v>72</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3">
         <v>47</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3">
-        <v>432</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1266,6 +1197,202 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
+  <cols>
+    <col min="1" max="1" width="29.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="37.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="86.1" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3">
+        <v>69</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3">
+        <v>71</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3">
+        <v>331</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3">
+        <v>332</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3">
+        <v>363</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3">
+        <v>390</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3">
+        <v>432</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3">
+        <v>439</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3">
+        <v>412</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3">
+        <v>72</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3">
+        <v>47</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:E1048576"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BEBB56A-E374-D240-A2E8-D1EA53AE5864}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1326,7 +1453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B33013-4172-2E43-B04F-F034BA65B290}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -1394,12 +1521,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD6C01A-77D7-8444-AC38-2E46178102DB}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1455,20 +1582,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="84">
+    <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="147">
+    <row r="7" spans="1:4" ht="110.25">
       <c r="A7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="12" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="63">
+      <c r="B9" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1476,6 +1608,10 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:D1048576"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="sinkiat.seow@vflowtech.com" xr:uid="{3EF89378-F192-43B3-925E-54E29E3B9FCE}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{F9CD1DE4-800A-452E-A512-D872EC69A950}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Missed out Excel sheet update
</commit_message>
<xml_diff>
--- a/Continuous Execution/vft_config.xlsx
+++ b/Continuous Execution/vft_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[01] Laptop Files\[01] School Files\Internship\[01] Work\[01] IoT\[01] IoT Devices\[04] Intern-IoT-Automated-Daily-Status (Github)\Continuous Execution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620393FE-2DFF-45A1-B4DA-227CB5C0EB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE2F69E-0EB5-4B2F-AE6B-8795E3E085EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6105" yWindow="1110" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>5kW - Unit 1 Backup 2</t>
   </si>
@@ -643,13 +643,10 @@
     <t>RECIPIENTS_DAILY</t>
   </si>
   <si>
-    <t>sinkiat.seow@vflowtech.com</t>
-  </si>
-  <si>
     <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com, saravanan.sampath@vflowtech.com, hardik.kansara@vflowtech.com, sanjana.ramesh@vflowtech.com, anhtrung.ta@vflowtech.com</t>
   </si>
   <si>
-    <t>vft.iot.test@gmail.com, john.jacob@vflowtech.com,
+    <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com,
 anhtrung.ta@vflowtech.com</t>
   </si>
 </sst>
@@ -761,6 +758,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -769,12 +772,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1103,7 +1100,7 @@
     <col min="2" max="2" width="35.875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.875" style="3" customWidth="1"/>
     <col min="4" max="4" width="37.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="35.5" style="11" customWidth="1"/>
     <col min="6" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
@@ -1120,7 +1117,7 @@
       <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1210,7 +1207,7 @@
     <col min="2" max="2" width="35.875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.875" style="3" customWidth="1"/>
     <col min="4" max="4" width="37.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="35.5" style="11" customWidth="1"/>
     <col min="6" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
@@ -1227,7 +1224,7 @@
       <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1408,10 +1405,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
@@ -1465,18 +1462,18 @@
   <cols>
     <col min="1" max="1" width="37.625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.875" style="2"/>
-    <col min="4" max="4" width="35.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="35.5" style="11" customWidth="1"/>
     <col min="5" max="5" width="10.875" style="2"/>
     <col min="6" max="6" width="35.5" style="5" customWidth="1"/>
     <col min="7" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="13"/>
+      <c r="D1" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1525,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD6C01A-77D7-8444-AC38-2E46178102DB}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1534,16 +1531,16 @@
     <col min="1" max="1" width="37.625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.375" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="35.5" style="11" customWidth="1"/>
     <col min="5" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="13"/>
+      <c r="D1" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1582,26 +1579,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="63">
       <c r="A6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>57</v>
+      <c r="B6" s="9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="110.25">
       <c r="A7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="63">
-      <c r="B9" s="13" t="s">
-        <v>59</v>
-      </c>
+      <c r="B7" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1610,7 +1605,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="sinkiat.seow@vflowtech.com" xr:uid="{3EF89378-F192-43B3-925E-54E29E3B9FCE}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{F9CD1DE4-800A-452E-A512-D872EC69A950}"/>
+    <hyperlink ref="B6" r:id="rId2" display="sinkiat.seow@vflowtech.com" xr:uid="{F9CD1DE4-800A-452E-A512-D872EC69A950}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update with sleep and mislabelling of CT1 Unit
</commit_message>
<xml_diff>
--- a/Continuous Execution/vft_config.xlsx
+++ b/Continuous Execution/vft_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[01] Laptop Files\[01] School Files\Internship\[01] Work\[01] IoT\[01] IoT Devices\[04] Intern-IoT-Automated-Daily-Status (Github)\Continuous Execution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[01] Laptop Files\[01] School Files\Internship\[01] Work\[01] IoT\[01] IoT Devices\[04] Automated Units Status (Bitbucket)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE2F69E-0EB5-4B2F-AE6B-8795E3E085EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E4144E-3FDE-4011-853C-ED839292FAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="1110" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
     <sheet name="closely_monitor_units_sheet" sheetId="5" r:id="rId1"/>
@@ -40,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
-  <si>
-    <t>5kW - Unit 1 Backup 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>5kW - Unit 4</t>
   </si>
@@ -133,9 +130,6 @@
     </r>
   </si>
   <si>
-    <t>Yet to deploy</t>
-  </si>
-  <si>
     <t>Email Fields</t>
   </si>
   <si>
@@ -643,11 +637,29 @@
     <t>RECIPIENTS_DAILY</t>
   </si>
   <si>
-    <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com, saravanan.sampath@vflowtech.com, hardik.kansara@vflowtech.com, sanjana.ramesh@vflowtech.com, anhtrung.ta@vflowtech.com</t>
-  </si>
-  <si>
     <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com,
 anhtrung.ta@vflowtech.com</t>
+  </si>
+  <si>
+    <t>10kW - Unit 7</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>5kW - Unit 1 Backup 1</t>
+  </si>
+  <si>
+    <t>5kW - Unit 2</t>
+  </si>
+  <si>
+    <t>Not Yet Online</t>
+  </si>
+  <si>
+    <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com, saravanan.sampath@vflowtech.com, hardik.kansara@vflowtech.com, sanjana.ramesh@vflowtech.com, anhtrung.ta@vflowtech.com, arjun.bhattarai@vflowtech.com, waikuan.loh@vflowtech.com</t>
+  </si>
+  <si>
+    <t>SG - CT1</t>
   </si>
 </sst>
 </file>
@@ -1106,19 +1118,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="86.1" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1126,13 +1138,13 @@
         <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1140,13 +1152,13 @@
         <v>363</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1154,13 +1166,13 @@
         <v>390</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1168,10 +1180,10 @@
         <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1179,10 +1191,10 @@
         <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1195,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1213,172 +1225,191 @@
   <sheetData>
     <row r="1" spans="1:5" ht="86.1" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3">
-        <v>331</v>
+        <v>71</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3">
-        <v>363</v>
+        <v>332</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3">
-        <v>390</v>
+        <v>363</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3">
-        <v>432</v>
+        <v>389</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3">
-        <v>439</v>
+        <v>390</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3">
-        <v>412</v>
+        <v>432</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>54</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3">
-        <v>72</v>
+        <v>439</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3">
+        <v>412</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3">
+        <v>72</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3">
         <v>47</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>47</v>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1406,40 +1437,40 @@
   <sheetData>
     <row r="1" spans="1:2" ht="31.5">
       <c r="A1" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1470,16 +1501,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="31.5">
       <c r="A1" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="13"/>
       <c r="D1" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
@@ -1487,7 +1518,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>30</v>
@@ -1495,7 +1526,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>1000</v>
@@ -1503,7 +1534,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -1522,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD6C01A-77D7-8444-AC38-2E46178102DB}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1537,24 +1568,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="31.5">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="13"/>
       <c r="D1" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6">
         <v>465</v>
@@ -1562,37 +1593,37 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="105">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="63">
       <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="110.25">
+    </row>
+    <row r="7" spans="1:4" ht="141.75">
       <c r="A7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4">

</xml_diff>

<commit_message>
Update continuous execution code
</commit_message>
<xml_diff>
--- a/Continuous Execution/vft_config.xlsx
+++ b/Continuous Execution/vft_config.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SorinoSK\School\Internship\Work\IoT\automated_units_status\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[01] Laptop Files\[01] School Files\Internship\[01] Work\[01] IoT\[01] IoT Devices\[04] Automated Units Status (Bitbucket)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665785E3-FFE9-4A78-9D8B-FDDF17024E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E4144E-3FDE-4011-853C-ED839292FAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
-    <sheet name="units_sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="account_sheet" sheetId="3" r:id="rId2"/>
-    <sheet name="data_sheet" sheetId="2" r:id="rId3"/>
-    <sheet name="email_sheet" sheetId="4" r:id="rId4"/>
+    <sheet name="closely_monitor_units_sheet" sheetId="5" r:id="rId1"/>
+    <sheet name="daily_report_units_sheet" sheetId="1" r:id="rId2"/>
+    <sheet name="account_sheet" sheetId="3" r:id="rId3"/>
+    <sheet name="data_sheet" sheetId="2" r:id="rId4"/>
+    <sheet name="email_sheet" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
-  <si>
-    <t>5kW - Unit 1 Backup 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>5kW - Unit 4</t>
   </si>
@@ -132,9 +130,6 @@
     </r>
   </si>
   <si>
-    <t>Yet to deploy</t>
-  </si>
-  <si>
     <t>Email Fields</t>
   </si>
   <si>
@@ -642,21 +637,36 @@
     <t>RECIPIENTS_DAILY</t>
   </si>
   <si>
-    <t>vft.iot.test@gmail.com,
-sinkiat.seow@vflowtech.com, john.jacob@vflowtech.com,
+    <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com,
 anhtrung.ta@vflowtech.com</t>
   </si>
   <si>
-    <t>vft.iot.test@gmail.com,
-sinkiat.seow@vflowtech.com, john.jacob@vflowtech.com, saravanan.sampath@vflowtech.com, hardik.kansara@vflowtech.com, sanjana.ramesh@vflowtech.com,
-anhtrung.ta@vflowtech.com</t>
+    <t>10kW - Unit 7</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>5kW - Unit 1 Backup 1</t>
+  </si>
+  <si>
+    <t>5kW - Unit 2</t>
+  </si>
+  <si>
+    <t>Not Yet Online</t>
+  </si>
+  <si>
+    <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com, saravanan.sampath@vflowtech.com, hardik.kansara@vflowtech.com, sanjana.ramesh@vflowtech.com, anhtrung.ta@vflowtech.com, arjun.bhattarai@vflowtech.com, waikuan.loh@vflowtech.com</t>
+  </si>
+  <si>
+    <t>SG - CT1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -710,6 +720,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -728,10 +746,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -751,6 +770,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -761,7 +786,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1073,11 +1099,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2916DAA6-D9E6-4FF8-8C3E-F0600BF95911}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1086,36 +1112,36 @@
     <col min="2" max="2" width="35.875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.875" style="3" customWidth="1"/>
     <col min="4" max="4" width="37.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="35.5" style="11" customWidth="1"/>
     <col min="6" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="86.1" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>21</v>
@@ -1123,138 +1149,52 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3">
-        <v>28</v>
+        <v>363</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3">
-        <v>71</v>
+        <v>390</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3">
-        <v>331</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3">
-        <v>332</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3">
-        <v>363</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3">
-        <v>390</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3">
-        <v>439</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3">
-        <v>412</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3">
-        <v>72</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3">
-        <v>47</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3">
-        <v>432</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1266,6 +1206,221 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
+  <cols>
+    <col min="1" max="1" width="29.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="37.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="86.1" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3">
+        <v>70</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3">
+        <v>69</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3">
+        <v>71</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3">
+        <v>331</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3">
+        <v>332</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3">
+        <v>363</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3">
+        <v>389</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3">
+        <v>390</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3">
+        <v>432</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3">
+        <v>439</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3">
+        <v>412</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3">
+        <v>72</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3">
+        <v>47</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:E1048576"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BEBB56A-E374-D240-A2E8-D1EA53AE5864}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1281,41 +1436,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5">
-      <c r="A1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="10"/>
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1326,7 +1481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B33013-4172-2E43-B04F-F034BA65B290}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -1338,24 +1493,24 @@
   <cols>
     <col min="1" max="1" width="37.625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.875" style="2"/>
-    <col min="4" max="4" width="35.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="35.5" style="11" customWidth="1"/>
     <col min="5" max="5" width="10.875" style="2"/>
     <col min="6" max="6" width="35.5" style="5" customWidth="1"/>
     <col min="7" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5">
-      <c r="A1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="D1" s="9" t="s">
-        <v>32</v>
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="D1" s="11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
@@ -1363,7 +1518,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>30</v>
@@ -1371,7 +1526,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>1000</v>
@@ -1379,7 +1534,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -1394,12 +1549,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD6C01A-77D7-8444-AC38-2E46178102DB}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1407,30 +1562,30 @@
     <col min="1" max="1" width="37.625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.375" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="35.5" style="11" customWidth="1"/>
     <col min="5" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5">
-      <c r="A1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="D1" s="9" t="s">
-        <v>37</v>
+      <c r="A1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="D1" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6">
         <v>465</v>
@@ -1438,44 +1593,51 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="105">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="84">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="63">
       <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="147">
+    </row>
+    <row r="7" spans="1:4" ht="141.75">
       <c r="A7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>58</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:D1048576"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="sinkiat.seow@vflowtech.com" xr:uid="{3EF89378-F192-43B3-925E-54E29E3B9FCE}"/>
+    <hyperlink ref="B6" r:id="rId2" display="sinkiat.seow@vflowtech.com" xr:uid="{F9CD1DE4-800A-452E-A512-D872EC69A950}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added verification email and modified dataplicity status read
</commit_message>
<xml_diff>
--- a/Continuous Execution/vft_config.xlsx
+++ b/Continuous Execution/vft_config.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[01] Laptop Files\[01] School Files\Internship\[01] Work\[01] IoT\[01] IoT Devices\[04] Automated Units Status (Bitbucket)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[01] Laptop Files\[06] Internship\[01] Work\[01] IoT\[01] IoT Devices\[04] Intern-IoT-Automated-Daily-Status (Github)\Continuous Execution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E4144E-3FDE-4011-853C-ED839292FAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3403E9-F3D3-4E5F-8C35-15CA5A719162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
-    <sheet name="closely_monitor_units_sheet" sheetId="5" r:id="rId1"/>
+    <sheet name="hourly_report_units_sheet" sheetId="5" r:id="rId1"/>
     <sheet name="daily_report_units_sheet" sheetId="1" r:id="rId2"/>
     <sheet name="account_sheet" sheetId="3" r:id="rId3"/>
     <sheet name="data_sheet" sheetId="2" r:id="rId4"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>5kW - Unit 4</t>
   </si>
@@ -89,9 +89,6 @@
     <t>100kW - Unit 10</t>
   </si>
   <si>
-    <t>5kW - Unit 0</t>
-  </si>
-  <si>
     <t>VFT_LOGIN_EMAIL</t>
   </si>
   <si>
@@ -108,12 +105,6 @@
   </si>
   <si>
     <t>No SIM</t>
-  </si>
-  <si>
-    <t>Data lagging</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
   </si>
   <si>
     <r>
@@ -523,9 +514,6 @@
     <t>SG - CT3</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>SG - Palau Ubin</t>
   </si>
   <si>
@@ -659,7 +647,7 @@
     <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com, saravanan.sampath@vflowtech.com, hardik.kansara@vflowtech.com, sanjana.ramesh@vflowtech.com, anhtrung.ta@vflowtech.com, arjun.bhattarai@vflowtech.com, waikuan.loh@vflowtech.com</t>
   </si>
   <si>
-    <t>SG - CT1</t>
+    <t>Indonesia</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2916DAA6-D9E6-4FF8-8C3E-F0600BF95911}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1124,13 +1112,13 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1141,10 +1129,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1155,46 +1143,51 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3">
-        <v>72</v>
+        <v>390</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3">
+        <v>72</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3">
         <v>47</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>45</v>
+      <c r="C7" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1207,10 +1200,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1231,63 +1224,66 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3">
-        <v>71</v>
+        <v>331</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>20</v>
@@ -1295,121 +1291,110 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3">
-        <v>332</v>
+        <v>363</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3">
-        <v>363</v>
+        <v>389</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3">
-        <v>390</v>
+        <v>432</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3">
-        <v>439</v>
+        <v>412</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3">
-        <v>412</v>
+        <v>72</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="3">
-        <v>47</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1443,34 +1428,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1486,7 +1471,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1505,7 +1490,7 @@
       </c>
       <c r="B1" s="13"/>
       <c r="D1" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1513,7 +1498,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1521,7 +1506,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1553,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD6C01A-77D7-8444-AC38-2E46178102DB}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1568,24 +1553,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="31.5">
       <c r="A1" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B1" s="13"/>
       <c r="D1" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" s="6">
         <v>465</v>
@@ -1593,37 +1578,37 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="105">
       <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="63">
       <c r="A6" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="141.75">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4">

</xml_diff>

<commit_message>
Update status pull logic
</commit_message>
<xml_diff>
--- a/Continuous Execution/vft_config.xlsx
+++ b/Continuous Execution/vft_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[01] Laptop Files\[06] Internship\[01] Work\[01] IoT\[01] IoT Devices\[04] Intern-IoT-Automated-Daily-Status (Github)\Continuous Execution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3403E9-F3D3-4E5F-8C35-15CA5A719162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F853C2-44B3-458A-AB38-F4685CA03624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{8D172AA6-0848-BB43-9F68-542271628B47}"/>
   </bookViews>
   <sheets>
     <sheet name="hourly_report_units_sheet" sheetId="5" r:id="rId1"/>
@@ -625,10 +625,6 @@
     <t>RECIPIENTS_DAILY</t>
   </si>
   <si>
-    <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com,
-anhtrung.ta@vflowtech.com</t>
-  </si>
-  <si>
     <t>10kW - Unit 7</t>
   </si>
   <si>
@@ -644,10 +640,13 @@
     <t>Not Yet Online</t>
   </si>
   <si>
-    <t>sinkiat.seow@vflowtech.com, vft.iot.test@gmail.com, john.jacob@vflowtech.com, saravanan.sampath@vflowtech.com, hardik.kansara@vflowtech.com, sanjana.ramesh@vflowtech.com, anhtrung.ta@vflowtech.com, arjun.bhattarai@vflowtech.com, waikuan.loh@vflowtech.com</t>
-  </si>
-  <si>
     <t>Indonesia</t>
+  </si>
+  <si>
+    <t>sinkiat.seow@vflowtech.com</t>
+  </si>
+  <si>
+    <t>sinkiat.seow@vflowtech.com, s.sinkiat@outlook.sg</t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1150,10 @@
         <v>389</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1202,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6952B871-99E0-F341-BE0D-6033E27DBDAB}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1238,7 +1237,7 @@
         <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>38</v>
@@ -1252,7 +1251,7 @@
         <v>69</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>38</v>
@@ -1319,10 +1318,10 @@
         <v>389</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1347,7 +1346,7 @@
         <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1361,7 +1360,7 @@
         <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1372,7 +1371,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1538,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD6C01A-77D7-8444-AC38-2E46178102DB}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
@@ -1595,20 +1594,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="63">
+    <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="141.75">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="31.5">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1621,7 +1620,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="sinkiat.seow@vflowtech.com" xr:uid="{3EF89378-F192-43B3-925E-54E29E3B9FCE}"/>
-    <hyperlink ref="B6" r:id="rId2" display="sinkiat.seow@vflowtech.com" xr:uid="{F9CD1DE4-800A-452E-A512-D872EC69A950}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{F9CD1DE4-800A-452E-A512-D872EC69A950}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>